<commit_message>
Test cases for Admin Tool section-Invoice Lookup is added
</commit_message>
<xml_diff>
--- a/bin/com/NFHS/xls/Suite.xlsx
+++ b/bin/com/NFHS/xls/Suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Description</t>
   </si>
@@ -57,9 +57,6 @@
     <t>My Courses distribution description</t>
   </si>
   <si>
-    <t>YES</t>
-  </si>
-  <si>
     <t>NO</t>
   </si>
   <si>
@@ -76,6 +73,18 @@
   </si>
   <si>
     <t>UserDashboard</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Tools</t>
+  </si>
+  <si>
+    <t>Admin Tools Scenarios</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -419,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -451,7 +460,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -462,7 +471,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -473,7 +482,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -484,7 +493,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -495,40 +504,51 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>